<commit_message>
Changes to accomodate new input template process such as new tab names
</commit_message>
<xml_diff>
--- a/output_file.xlsx
+++ b/output_file.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="62">
   <si>
     <t>AsOfDate</t>
   </si>
@@ -34,10 +34,10 @@
     <t>IndexWeight</t>
   </si>
   <si>
-    <t>9/30/2019</t>
-  </si>
-  <si>
-    <t>MSAUM</t>
+    <t>3/31/2021</t>
+  </si>
+  <si>
+    <t>MSMUA</t>
   </si>
   <si>
     <t>Communication Services</t>
@@ -73,9 +73,6 @@
     <t>Utilities</t>
   </si>
   <si>
-    <t>[Unassigned]</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -88,22 +85,19 @@
     <t>SimWeight</t>
   </si>
   <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>&gt; A$100B</t>
-  </si>
-  <si>
-    <t>A$25B - A$100B</t>
-  </si>
-  <si>
-    <t>A$15B - A$25B</t>
-  </si>
-  <si>
-    <t>A$2B - A$15B</t>
-  </si>
-  <si>
-    <t>&lt; A$2B</t>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>&gt; $100B</t>
+  </si>
+  <si>
+    <t>$25B - $100B</t>
+  </si>
+  <si>
+    <t>$15B - $25B</t>
+  </si>
+  <si>
+    <t>$2B - $15B</t>
   </si>
   <si>
     <t>Char</t>
@@ -136,40 +130,40 @@
     <t>Weighted Median Market Cap</t>
   </si>
   <si>
-    <t>21.90</t>
-  </si>
-  <si>
-    <t>4.50%</t>
-  </si>
-  <si>
-    <t>10.19%</t>
-  </si>
-  <si>
-    <t>2.53</t>
-  </si>
-  <si>
-    <t>A$58.9 B</t>
-  </si>
-  <si>
-    <t>A$27.1 B</t>
-  </si>
-  <si>
-    <t>22.60</t>
-  </si>
-  <si>
-    <t>4.53%</t>
-  </si>
-  <si>
-    <t>6.61%</t>
-  </si>
-  <si>
-    <t>2.51</t>
-  </si>
-  <si>
-    <t>A$68.4 B</t>
-  </si>
-  <si>
-    <t>A$45.1 B</t>
+    <t>30.79</t>
+  </si>
+  <si>
+    <t>1.87%</t>
+  </si>
+  <si>
+    <t>12.17%</t>
+  </si>
+  <si>
+    <t>6.59</t>
+  </si>
+  <si>
+    <t>$101.5 B</t>
+  </si>
+  <si>
+    <t>$62.3 B</t>
+  </si>
+  <si>
+    <t>31.49</t>
+  </si>
+  <si>
+    <t>2.03%</t>
+  </si>
+  <si>
+    <t>11.92%</t>
+  </si>
+  <si>
+    <t>6.47</t>
+  </si>
+  <si>
+    <t>$146.1 B</t>
+  </si>
+  <si>
+    <t>$62.0 B</t>
   </si>
   <si>
     <t>Holding</t>
@@ -181,34 +175,34 @@
     <t>WeightSum</t>
   </si>
   <si>
-    <t>BHP Group Ltd</t>
-  </si>
-  <si>
-    <t>Woolworths Group Ltd</t>
-  </si>
-  <si>
-    <t>Commonwealth Bank of Australia</t>
-  </si>
-  <si>
-    <t>Transurban Group Ltd.</t>
-  </si>
-  <si>
-    <t>Rio Tinto Limited</t>
-  </si>
-  <si>
-    <t>Newcrest Mining Limited</t>
-  </si>
-  <si>
-    <t>Goodman Group</t>
-  </si>
-  <si>
-    <t>Brambles Limited</t>
-  </si>
-  <si>
-    <t>Telstra Corporation Limited</t>
-  </si>
-  <si>
-    <t>Fortescue Metals Group Ltd</t>
+    <t>Accenture Plc Class A</t>
+  </si>
+  <si>
+    <t>Progressive Corporation</t>
+  </si>
+  <si>
+    <t>Bristol-Myers Squibb Company</t>
+  </si>
+  <si>
+    <t>Crown Castle International Corp</t>
+  </si>
+  <si>
+    <t>International Business Machines Corporation</t>
+  </si>
+  <si>
+    <t>Johnson &amp; Johnson</t>
+  </si>
+  <si>
+    <t>McCormick &amp; Company, Incorporated</t>
+  </si>
+  <si>
+    <t>Target Corporation</t>
+  </si>
+  <si>
+    <t>Citrix Systems, Inc.</t>
+  </si>
+  <si>
+    <t>Campbell Soup Company</t>
   </si>
 </sst>
 </file>
@@ -571,7 +565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -609,10 +603,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>0.0439235729215636</v>
+        <v>0.0368403787726158</v>
       </c>
       <c r="E2" s="2">
-        <v>0.0159049275762766</v>
+        <v>0.092436059678063</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -626,10 +620,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>0.0340146451110033</v>
+        <v>0.09587812042528819</v>
       </c>
       <c r="E3" s="2">
-        <v>0.0571115552002986</v>
+        <v>0.0660985814489681</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -643,10 +637,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <v>0.0706612308434075</v>
+        <v>0.156846905704609</v>
       </c>
       <c r="E4" s="2">
-        <v>0.0577709113866651</v>
+        <v>0.110359306949875</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -663,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>0.0566751291598808</v>
+        <v>0.00251022935405877</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -677,10 +671,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="2">
-        <v>0.176151885741071</v>
+        <v>0.0987685566128636</v>
       </c>
       <c r="E6" s="2">
-        <v>0.385883065797229</v>
+        <v>0.08954457073348471</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -694,10 +688,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="2">
-        <v>0.0438320531053649</v>
+        <v>0.147171183234493</v>
       </c>
       <c r="E7" s="2">
-        <v>0.0979915328995476</v>
+        <v>0.188164239643132</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -711,10 +705,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="2">
-        <v>0.175828240194404</v>
+        <v>0.0730501749977322</v>
       </c>
       <c r="E8" s="2">
-        <v>0.06137602629616121</v>
+        <v>0.0776590703465664</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -728,10 +722,10 @@
         <v>14</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <v>0.292843039869761</v>
       </c>
       <c r="E9" s="2">
-        <v>0.00548403060557182</v>
+        <v>0.235251101220946</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -745,10 +739,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="2">
-        <v>0.22272062625372</v>
+        <v>0.0257900336337672</v>
       </c>
       <c r="E10" s="2">
-        <v>0.164960849871498</v>
+        <v>0.0280231271238259</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -762,10 +756,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="2">
-        <v>0.18496399679086</v>
+        <v>0.0477916390022694</v>
       </c>
       <c r="E11" s="2">
-        <v>0.0764106268724576</v>
+        <v>0.0344293370513692</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -779,27 +773,10 @@
         <v>17</v>
       </c>
       <c r="D12" s="2">
-        <v>0.0479037490386058</v>
+        <v>0.0250199677466008</v>
       </c>
       <c r="E12" s="2">
-        <v>0.0204313443344136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
+        <v>0.07552437644971109</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +786,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -827,16 +804,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -850,19 +827,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2">
-        <v>0.271756547733519</v>
+        <v>0.38758510319214</v>
       </c>
       <c r="G2" s="2">
-        <v>0.343094235570015</v>
+        <v>0.370893687603703</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -873,19 +850,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2">
-        <v>0.369919004980053</v>
+        <v>0.387982644642594</v>
       </c>
       <c r="G3" s="2">
-        <v>0.309233968873235</v>
+        <v>0.454372528558921</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -896,19 +873,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
-        <v>0.102556894319319</v>
+        <v>0.163760518702805</v>
       </c>
       <c r="G4" s="2">
-        <v>0.114274839986842</v>
+        <v>0.104664363648447</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -919,42 +896,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2">
-        <v>0.255767552967109</v>
+        <v>0.06067173346246151</v>
       </c>
       <c r="G5" s="2">
-        <v>0.233396955569908</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>4.790944530302851E-05</v>
+        <v>0.0700694201889292</v>
       </c>
     </row>
   </sheetData>
@@ -983,16 +937,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1003,16 +957,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="F2" s="1">
-        <v>68</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1023,16 +977,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1043,16 +997,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1063,16 +1017,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1083,16 +1037,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1103,16 +1057,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1123,16 +1077,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1160,13 +1114,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1177,13 +1131,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
-        <v>0.0713439838326147</v>
+        <v>0.0581071909668409</v>
       </c>
       <c r="E2" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1194,13 +1148,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2">
-        <v>0.0665952919987516</v>
+        <v>0.0468109429178378</v>
       </c>
       <c r="E3" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1211,13 +1165,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2">
-        <v>0.0663242661415949</v>
+        <v>0.04056710513628339</v>
       </c>
       <c r="E4" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1228,13 +1182,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2">
-        <v>0.0634697988660864</v>
+        <v>0.0374801068532375</v>
       </c>
       <c r="E5" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1245,13 +1199,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2">
-        <v>0.0548463836909889</v>
+        <v>0.0314563481697103</v>
       </c>
       <c r="E6" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1262,13 +1216,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2">
-        <v>0.0527351774494144</v>
+        <v>0.0268942334700008</v>
       </c>
       <c r="E7" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1279,13 +1233,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2">
-        <v>0.0525171868105171</v>
+        <v>0.0264738775025792</v>
       </c>
       <c r="E8" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1296,13 +1250,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2">
-        <v>0.04868752402234459</v>
+        <v>0.0261026620817259</v>
       </c>
       <c r="E9" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1313,13 +1267,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2">
-        <v>0.0439235729215636</v>
+        <v>0.0247964746261889</v>
       </c>
       <c r="E10" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1330,13 +1284,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2">
-        <v>0.04379508128070179</v>
+        <v>0.0246477471128067</v>
       </c>
       <c r="E11" s="2">
-        <v>0.5642382670145779</v>
+        <v>0.3433366888372114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>